<commit_message>
Stand 28.10.2020 22:00 korrigiert
</commit_message>
<xml_diff>
--- a/Covid19DUS.xlsx
+++ b/Covid19DUS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dirk/Documents/Covid19DUS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6247A2D-618B-1945-955A-D550B660CD0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8DBDF5-60CB-6C47-92A0-D6D5D3E1F94C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27900" windowHeight="26820" xr2:uid="{D96A2E1C-F68D-7A4E-A558-DE7788A0A4F9}"/>
   </bookViews>
@@ -7168,7 +7168,7 @@
                   <c:v>674</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>755</c:v>
+                  <c:v>810</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8521,7 +8521,7 @@
                   <c:v>4451</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>4576</c:v>
+                  <c:v>4521</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13630,7 +13630,7 @@
                   <c:v>674</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>755</c:v>
+                  <c:v>810</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14981,7 +14981,7 @@
                   <c:v>4451</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>4576</c:v>
+                  <c:v>4521</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20090,7 +20090,7 @@
                   <c:v>674</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>755</c:v>
+                  <c:v>810</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -23244,8 +23244,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:S222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F164" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q222" sqref="Q222"/>
+    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K220" sqref="K220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -35610,7 +35610,7 @@
         <v>229</v>
       </c>
       <c r="Q215" s="20">
-        <f>SUM(O209:O215)/$Q$1</f>
+        <f t="shared" ref="Q215:Q220" si="4">SUM(O209:O215)/$Q$1</f>
         <v>107.13351281809132</v>
       </c>
       <c r="R215" s="2">
@@ -35670,7 +35670,7 @@
         <v>0</v>
       </c>
       <c r="Q216" s="20">
-        <f>SUM(O210:O216)/$Q$1</f>
+        <f t="shared" si="4"/>
         <v>94.283683968522567</v>
       </c>
       <c r="R216" s="2">
@@ -35733,7 +35733,7 @@
         <v>54</v>
       </c>
       <c r="Q217" s="20">
-        <f>SUM(O211:O217)/$Q$1</f>
+        <f t="shared" si="4"/>
         <v>130.82054672151324</v>
       </c>
       <c r="R217" s="2">
@@ -35793,7 +35793,7 @@
         <v>35</v>
       </c>
       <c r="Q218" s="20">
-        <f>SUM(O212:O218)/$Q$1</f>
+        <f t="shared" si="4"/>
         <v>145.99263379690768</v>
       </c>
       <c r="R218" s="2">
@@ -35853,7 +35853,7 @@
         <v>160</v>
       </c>
       <c r="Q219" s="20">
-        <f>SUM(O213:O219)/$Q$1</f>
+        <f t="shared" si="4"/>
         <v>154.35276340988014</v>
       </c>
       <c r="R219" s="2">
@@ -35883,16 +35883,16 @@
       </c>
       <c r="H220" s="11">
         <f>CD[[#This Row],[Infiziert]]-CD[[#This Row],[KH (nicht intensiv)]]-CD[[#This Row],[KH (intensiv)]]</f>
-        <v>755</v>
+        <v>810</v>
       </c>
       <c r="I220" s="10">
-        <v>4576</v>
+        <v>4521</v>
       </c>
       <c r="J220" s="10">
         <v>5496</v>
       </c>
       <c r="K220" s="10">
-        <v>865</v>
+        <v>920</v>
       </c>
       <c r="L220" s="10">
         <v>110</v>
@@ -35910,10 +35910,10 @@
       </c>
       <c r="P220" s="12">
         <f>CD[[#This Row],[Genesen]]-I219</f>
-        <v>125</v>
+        <v>70</v>
       </c>
       <c r="Q220" s="20">
-        <f>SUM(O214:O220)/$Q$1</f>
+        <f t="shared" si="4"/>
         <v>172.00192592615528</v>
       </c>
       <c r="R220" s="2">

</xml_diff>

<commit_message>
inkl. Krankenhaus-Zahlen vom 12.02.2021
</commit_message>
<xml_diff>
--- a/Covid19DUS.xlsx
+++ b/Covid19DUS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dirk/Documents/Covid19DUS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826BFE1A-2441-FA40-B091-097CEB8B6CE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D294272-9D64-EE49-927F-5F0AA7AEA56F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12100" yWindow="2220" windowWidth="38440" windowHeight="26580" xr2:uid="{D96A2E1C-F68D-7A4E-A558-DE7788A0A4F9}"/>
   </bookViews>
@@ -422,11 +422,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Berechnung" xfId="2" builtinId="22"/>
@@ -6818,7 +6818,7 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="323" formatCode="0">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8809,7 +8809,7 @@
                   <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="323">
-                  <c:v>67</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15260,7 +15260,7 @@
               <a:cs typeface="Helvetica Neue" panose="02000503000000020004" pitchFamily="2" charset="0"/>
             </a:rPr>
             <a:pPr algn="ctr"/>
-            <a:t>13.02., insg. 16.427 (+24) Düsseldorfer mit Coronadiagnose, akt. infiz.: 837 (-68), 83 (0) in Krankenhäusern i. Beh., davon 16 (0) auf Intensiv, 973 (0) in Quaran., 15.338 (+88) genesen. 252 (+4) verstorben, 7-Tages-Inzidenz 37,1 (42,3) #CoronaD</a:t>
+            <a:t>13.02., insg. 16.427 (+24) Düsseldorfer mit Coronadiagnose, akt. infiz.: 837 (-68), 90 (+7) in Krankenhäusern i. Beh., davon 15 (-1) auf Intensiv, 971 (-2) in Quaran., 15.338 (+88) genesen. 252 (+4) verstorben, 7-Tages-Inzidenz 37,1 (42,3) #CoronaD</a:t>
           </a:fld>
           <a:endParaRPr lang="de-DE" sz="900">
             <a:latin typeface="Helvetica Neue" panose="02000503000000020004" pitchFamily="2" charset="0"/>
@@ -15639,8 +15639,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:W342"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15666,12 +15666,12 @@
       <c r="F1" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
       <c r="L1" s="3" t="s">
         <v>22</v>
       </c>
@@ -15790,11 +15790,11 @@
       </c>
       <c r="V6" s="3" t="str" cm="1">
         <f t="array" ref="V6">TEXT(INDEX(CD[KH],$S$5),"#.##0")</f>
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="W6" s="3" t="str" cm="1">
         <f t="array" ref="W6">TEXT(INDEX(CD[KH],$S$5)-INDEX(CD[KH],$S$5-1),"+#.##0;-#.##0;0")</f>
-        <v>0</v>
+        <v>+7</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
@@ -15862,11 +15862,11 @@
       </c>
       <c r="V7" s="3" t="str" cm="1">
         <f t="array" ref="V7">TEXT(INDEX(CD[KH (intensiv)],$S$5),"#.##0")</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="W7" s="3" t="str" cm="1">
         <f t="array" ref="W7">TEXT(INDEX(CD[KH (intensiv)],$S$5)-INDEX(CD[KH (intensiv)],$S$5-1),"+#.##0;-#.##0;0")</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
@@ -15942,11 +15942,11 @@
       </c>
       <c r="V8" s="3" t="str" cm="1">
         <f t="array" ref="V8">TEXT(INDEX(CD[Quarant],$S$5),"#.##0")</f>
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="W8" s="3" t="str" cm="1">
         <f t="array" ref="W8">TEXT(INDEX(CD[Quarant],$S$5)-INDEX(CD[Quarant],$S$5-1),"+#.##0;-#.##0;0")</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
@@ -16276,7 +16276,7 @@
       </c>
       <c r="R13" s="18" t="str">
         <f ca="1">S6&amp;", insg. "&amp;S10&amp;" ("&amp;T10&amp;") Düsseldorfer mit Coronadiagnose, akt. infiz.: "&amp;S9&amp;" ("&amp;T9&amp;"), "&amp;V6&amp;" ("&amp;W6&amp;") in Krankenhäusern i. Beh., davon "&amp;V7&amp;" ("&amp;W7&amp;") auf Intensiv, "&amp;V8&amp;" ("&amp;W8&amp;") in Quaran., "&amp;V9&amp;" ("&amp;W9&amp;") genesen. "&amp;S8&amp;" ("&amp;T8&amp;") verstorben, 7-Tages-Inzidenz "&amp;S7&amp;" ("&amp;T7&amp;") #CoronaD"</f>
-        <v>13.02., insg. 16.427 (+24) Düsseldorfer mit Coronadiagnose, akt. infiz.: 837 (-68), 83 (0) in Krankenhäusern i. Beh., davon 16 (0) auf Intensiv, 973 (0) in Quaran., 15.338 (+88) genesen. 252 (+4) verstorben, 7-Tages-Inzidenz 37,1 (42,3) #CoronaD</v>
+        <v>13.02., insg. 16.427 (+24) Düsseldorfer mit Coronadiagnose, akt. infiz.: 837 (-68), 90 (+7) in Krankenhäusern i. Beh., davon 15 (-1) auf Intensiv, 971 (-2) in Quaran., 15.338 (+88) genesen. 252 (+4) verstorben, 7-Tages-Inzidenz 37,1 (42,3) #CoronaD</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
@@ -33974,7 +33974,7 @@
         <f>CD[[#This Row],[Total]]-I313</f>
         <v>140</v>
       </c>
-      <c r="O314" s="52">
+      <c r="O314" s="51">
         <f>CD[[#This Row],[Genesen]]-H313</f>
         <v>-17</v>
       </c>
@@ -34519,7 +34519,7 @@
         <f>CD[[#This Row],[Total]]-I322</f>
         <v>56</v>
       </c>
-      <c r="O323" s="52">
+      <c r="O323" s="51">
         <f>CD[[#This Row],[Genesen]]-H322</f>
         <v>-779</v>
       </c>
@@ -34914,16 +34914,16 @@
       <c r="D330" s="46">
         <v>252</v>
       </c>
-      <c r="E330" s="51">
-        <v>16</v>
+      <c r="E330" s="53">
+        <v>15</v>
       </c>
       <c r="F330" s="23">
         <f>CD[[#This Row],[KH]]-CD[[#This Row],[KH (intensiv)]]</f>
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="G330" s="23">
         <f>CD[[#This Row],[Infiziert]]-CD[[#This Row],[KH (nicht intensiv)]]-CD[[#This Row],[KH (intensiv)]]</f>
-        <v>754</v>
+        <v>747</v>
       </c>
       <c r="H330" s="48">
         <v>15338</v>
@@ -34934,11 +34934,11 @@
       <c r="J330" s="50">
         <v>837</v>
       </c>
-      <c r="K330" s="25">
-        <v>83</v>
-      </c>
-      <c r="L330" s="25">
-        <v>973</v>
+      <c r="K330" s="28">
+        <v>90</v>
+      </c>
+      <c r="L330" s="28">
+        <v>971</v>
       </c>
       <c r="M330" s="23">
         <f>CD[[#This Row],[Verstorbene]]+CD[[#This Row],[KH (intensiv)]]+CD[[#This Row],[KH (nicht intensiv)]]+CD[[#This Row],[Infiziert (o. KH)]]+CD[[#This Row],[Genesen]]-CD[[#This Row],[Total]]</f>

</xml_diff>